<commit_message>
added -ve mode and some more analysis
</commit_message>
<xml_diff>
--- a/notebooks/comparison_of_proportions_of_transformations_excluding_singletons.xlsx
+++ b/notebooks/comparison_of_proportions_of_transformations_excluding_singletons.xlsx
@@ -9,18 +9,33 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Positive mode" sheetId="1" r:id="rId1"/>
+    <sheet name="Negative mode" sheetId="2" r:id="rId2"/>
+    <sheet name="Pos Adduct Counts" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="batch1_Std_1_1_tran_counts" localSheetId="0">Sheet1!$F$3:$G$73</definedName>
-    <definedName name="batch1_Std_1_2_tran_counts" localSheetId="0">Sheet1!$H$3:$I$73</definedName>
-    <definedName name="batch1_Std_2_1_tran_counts" localSheetId="0">Sheet1!$J$3:$K$73</definedName>
-    <definedName name="batch1_Std_2_2_tran_counts" localSheetId="0">Sheet1!$L$3:$M$73</definedName>
-    <definedName name="Beer_3_Full1_tran_counts" localSheetId="0">Sheet1!$A$3:$C$73</definedName>
-    <definedName name="Urine_37_fullscan1_POS_tran_counts" localSheetId="0">Sheet1!$D$3:$E$73</definedName>
+    <definedName name="batch1_Std_1_1_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$C$2:$C$6</definedName>
+    <definedName name="batch1_Std_1_1_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$D$13:$E$18</definedName>
+    <definedName name="batch1_Std_1_1_tran_counts" localSheetId="0">'Positive mode'!$F$3:$G$73</definedName>
+    <definedName name="batch1_Std_1_2_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$D$2:$D$6</definedName>
+    <definedName name="batch1_Std_1_2_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$F$13:$G$18</definedName>
+    <definedName name="batch1_Std_1_2_tran_counts" localSheetId="0">'Positive mode'!$H$3:$I$73</definedName>
+    <definedName name="batch1_Std_2_1_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$E$2:$E$6</definedName>
+    <definedName name="batch1_Std_2_1_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$H$13:$I$18</definedName>
+    <definedName name="batch1_Std_2_1_tran_counts" localSheetId="0">'Positive mode'!$J$3:$K$73</definedName>
+    <definedName name="batch1_Std_2_2_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$F$2:$F$6</definedName>
+    <definedName name="batch1_Std_2_2_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$J$13:$K$18</definedName>
+    <definedName name="batch1_Std_2_2_tran_counts" localSheetId="0">'Positive mode'!$L$3:$M$73</definedName>
+    <definedName name="Beer_3_Full1_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$A$2:$B$6</definedName>
+    <definedName name="Beer_3_Full1_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$A$13:$C$18</definedName>
+    <definedName name="Beer_3_Full1_NEG_tran_counts" localSheetId="1">'Negative mode'!$A$3:$C$73</definedName>
+    <definedName name="Beer_3_Full1_tran_counts" localSheetId="0">'Positive mode'!$A$3:$C$73</definedName>
+    <definedName name="Urine_37_fullscan1_POS_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$G$2:$G$6</definedName>
+    <definedName name="Urine_37_fullscan1_POS_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$L$13:$M$18</definedName>
+    <definedName name="Urine_37_fullscan1_POS_tran_counts" localSheetId="0">'Positive mode'!$D$3:$E$73</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +48,25 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="batch1_Std_1_1_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="batch1_Std_1_1_adduct_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_1_1_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="batch1_Std_1_1_adduct_counts1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_1_1_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="batch1_Std_1_1_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_1_1_tran_counts.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -42,7 +75,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="batch1_Std_1_2_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="batch1_Std_1_2_adduct_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_1_2_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="batch1_Std_1_2_adduct_counts1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_1_2_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="batch1_Std_1_2_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_1_2_tran_counts.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -51,7 +102,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="batch1_Std_2_1_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="batch1_Std_2_1_adduct_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_2_1_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="batch1_Std_2_1_adduct_counts1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_2_1_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="batch1_Std_2_1_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_2_1_tran_counts.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -60,7 +129,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="batch1_Std_2_2_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="10" name="batch1_Std_2_2_adduct_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_2_2_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="11" name="batch1_Std_2_2_adduct_counts1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_2_2_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="12" name="batch1_Std_2_2_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/batch1_Std_2_2_tran_counts.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -69,7 +156,34 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="Beer_3_Full1_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="13" name="Beer_3_Full1_adduct_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/Beer_3_Full1_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="14" name="Beer_3_Full1_adduct_counts1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/Beer_3_Full1_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="15" name="Beer_3_Full1_NEG_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/Beer_3_Full1_NEG_tran_counts.txt" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="16" name="Beer_3_Full1_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/Beer_3_Full1_tran_counts.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -78,7 +192,25 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="Urine_37_fullscan1_POS_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="17" name="Urine_37_fullscan1_POS_adduct_counts" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/Urine_37_fullscan1_POS_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="18" name="Urine_37_fullscan1_POS_adduct_counts1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/Urine_37_fullscan1_POS_adduct_counts.txt" comma="1">
+      <textFields count="3">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="19" name="Urine_37_fullscan1_POS_tran_counts" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/simon/git/ms1fun/notebooks/Urine_37_fullscan1_POS_tran_counts.txt" comma="1">
       <textFields count="3">
         <textField/>
@@ -91,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="160">
   <si>
     <t>M+H</t>
   </si>
@@ -331,6 +463,246 @@
   </si>
   <si>
     <t>Std_2_2</t>
+  </si>
+  <si>
+    <t>M-H</t>
+  </si>
+  <si>
+    <t>M-H[C13]</t>
+  </si>
+  <si>
+    <t>M-H[2C13]</t>
+  </si>
+  <si>
+    <t>M+CH2O2-H</t>
+  </si>
+  <si>
+    <t>M+ACN-H</t>
+  </si>
+  <si>
+    <t>M+CH2O2-H[C13]</t>
+  </si>
+  <si>
+    <t>M+CH2O2-H[2C13]</t>
+  </si>
+  <si>
+    <t>M+ACN-H[C13]</t>
+  </si>
+  <si>
+    <t>M+ACN-H[2C13]</t>
+  </si>
+  <si>
+    <t>2M-H</t>
+  </si>
+  <si>
+    <t>[M-H2O]-H</t>
+  </si>
+  <si>
+    <t>[M-CO2]-H</t>
+  </si>
+  <si>
+    <t>[M-CO]-H</t>
+  </si>
+  <si>
+    <t>M-2H</t>
+  </si>
+  <si>
+    <t>M+NH3-H</t>
+  </si>
+  <si>
+    <t>2M-H[C13]</t>
+  </si>
+  <si>
+    <t>2M-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]-H[2C13]</t>
+  </si>
+  <si>
+    <t>M-2H[C13]</t>
+  </si>
+  <si>
+    <t>M-2H[2C13]</t>
+  </si>
+  <si>
+    <t>M+NH3-H[C13]</t>
+  </si>
+  <si>
+    <t>M+NH3-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]+CH2O2-H</t>
+  </si>
+  <si>
+    <t>[M-CO2]+CH2O2-H</t>
+  </si>
+  <si>
+    <t>[M-CO]+CH2O2-H</t>
+  </si>
+  <si>
+    <t>[M-H2O]+ACN-H</t>
+  </si>
+  <si>
+    <t>[M-CO2]+ACN-H</t>
+  </si>
+  <si>
+    <t>[M-CO]+ACN-H</t>
+  </si>
+  <si>
+    <t>[M-H2O]+CH2O2-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]+CH2O2-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]+CH2O2-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]+CH2O2-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]+CH2O2-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]+CH2O2-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]+ACN-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]+ACN-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]+ACN-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]+ACN-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]+ACN-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]+ACN-H[2C13]</t>
+  </si>
+  <si>
+    <t>[2M-H2O]-H</t>
+  </si>
+  <si>
+    <t>[2M-CO2]-H</t>
+  </si>
+  <si>
+    <t>[2M-CO]-H</t>
+  </si>
+  <si>
+    <t>[M-H2O]-H-H</t>
+  </si>
+  <si>
+    <t>[M-CO2]-H-H</t>
+  </si>
+  <si>
+    <t>[M-CO]-H-H</t>
+  </si>
+  <si>
+    <t>[M-H2O]+NH3-H</t>
+  </si>
+  <si>
+    <t>[M-CO2]+NH3-H</t>
+  </si>
+  <si>
+    <t>[M-CO]+NH3-H</t>
+  </si>
+  <si>
+    <t>[2M-H2O]-H[C13]</t>
+  </si>
+  <si>
+    <t>[2M-H2O]-H[2C13]</t>
+  </si>
+  <si>
+    <t>[2M-CO2]-H[C13]</t>
+  </si>
+  <si>
+    <t>[2M-CO2]-H[2C13]</t>
+  </si>
+  <si>
+    <t>[2M-CO]-H[C13]</t>
+  </si>
+  <si>
+    <t>[2M-CO]-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]-H-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]-H-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]-H-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]-H-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]-H-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]-H-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]+NH3-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-H2O]+NH3-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]+NH3-H[C13]</t>
+  </si>
+  <si>
+    <t>[M-CO2]+NH3-H[2C13]</t>
+  </si>
+  <si>
+    <t>[M-CO]+NH3-H[C13]</t>
+  </si>
+  <si>
+    <t>Adduct</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>CH2O2</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>ACN</t>
+  </si>
+  <si>
+    <t>CH3OH</t>
+  </si>
+  <si>
+    <t>NH4</t>
+  </si>
+  <si>
+    <t>Na</t>
   </si>
 </sst>
 </file>
@@ -366,11 +738,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +838,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$73</c:f>
+              <c:f>'Positive mode'!$A$3:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
@@ -686,7 +1059,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$73</c:f>
+              <c:f>'Positive mode'!$C$3:$C$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
@@ -925,7 +1298,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$73</c:f>
+              <c:f>'Positive mode'!$A$3:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
@@ -1146,7 +1519,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$73</c:f>
+              <c:f>'Positive mode'!$E$3:$E$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
@@ -1385,7 +1758,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$73</c:f>
+              <c:f>'Positive mode'!$G$3:$G$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
@@ -1624,7 +1997,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$73</c:f>
+              <c:f>'Positive mode'!$I$3:$I$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
@@ -1863,7 +2236,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$73</c:f>
+              <c:f>'Positive mode'!$K$3:$K$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
@@ -2102,7 +2475,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$73</c:f>
+              <c:f>'Positive mode'!$M$3:$M$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
@@ -2520,7 +2893,1546 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Negative mode'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Negative mode'!$A$3:$A$73</c:f>
+              <c:strCache>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>M-H</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>M-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>M-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>M+CH2O2-H</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>M+ACN-H</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>M+CH2O2-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>M+CH2O2-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>M+ACN-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>M+ACN-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2M-H</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>[M-H2O]-H</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>[M-CO2]-H</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>[M-CO]-H</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>M-2H</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>M+NH3-H</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2M-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2M-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>[M-H2O]-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>[M-H2O]-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>[M-CO2]-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>[M-CO2]-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>[M-CO]-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>[M-CO]-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>M-2H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>M-2H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>M+NH3-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>M+NH3-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>[M-H2O]+CH2O2-H</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>[M-CO2]+CH2O2-H</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>[M-CO]+CH2O2-H</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>[M-H2O]+ACN-H</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>[M-CO2]+ACN-H</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>[M-CO]+ACN-H</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>[M-H2O]+CH2O2-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>[M-H2O]+CH2O2-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>[M-CO2]+CH2O2-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>[M-CO2]+CH2O2-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>[M-CO]+CH2O2-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>[M-CO]+CH2O2-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>[M-H2O]+ACN-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>[M-H2O]+ACN-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>[M-CO2]+ACN-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>[M-CO2]+ACN-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>[M-CO]+ACN-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>[M-CO]+ACN-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>[2M-H2O]-H</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>[2M-CO2]-H</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>[2M-CO]-H</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>[M-H2O]-H-H</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>[M-CO2]-H-H</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>[M-CO]-H-H</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>[M-H2O]+NH3-H</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>[M-CO2]+NH3-H</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>[M-CO]+NH3-H</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>[2M-H2O]-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>[2M-H2O]-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>[2M-CO2]-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>[2M-CO2]-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>[2M-CO]-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>[2M-CO]-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>[M-H2O]-H-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>[M-H2O]-H-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>[M-CO2]-H-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>[M-CO2]-H-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>[M-CO]-H-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>[M-CO]-H-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>[M-H2O]+NH3-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>[M-H2O]+NH3-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>[M-CO2]+NH3-H[C13]</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>[M-CO2]+NH3-H[2C13]</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>[M-CO]+NH3-H[C13]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Negative mode'!$C$3:$C$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="71"/>
+                <c:pt idx="0">
+                  <c:v>0.3178</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0381</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0344</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.044</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0051</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0034</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0723</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0361</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0395</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.046</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0085</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0031</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0023</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.0008</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.013</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.0079</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.0268</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.0183</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.0164</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.0056</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.0087</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.0008</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.0034</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.0031</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.0006</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.0014</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.0003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.0008</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.0025</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.0031</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.0051</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.0025</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.0025</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.0017</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.0178</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.0054</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.011</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.0014</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.0003</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.0003</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.0006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2070310080"/>
+        <c:axId val="-2032344496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2070310080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2032344496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2032344496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2070310080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Adducts</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Beer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CH2O2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ACN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CH3OH</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NH4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Na</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pos Adduct Counts'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0139</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0359</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0321</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0493</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Std_1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CH2O2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ACN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CH3OH</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NH4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Na</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pos Adduct Counts'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0076</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0211</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0344</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Std_1_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CH2O2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ACN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CH3OH</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NH4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Na</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pos Adduct Counts'!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Std_2_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CH2O2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ACN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CH3OH</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NH4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Na</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pos Adduct Counts'!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0205</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0184</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0263</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Std_2_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CH2O2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ACN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CH3OH</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NH4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Na</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pos Adduct Counts'!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0214</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0259</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0319</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Urine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pos Adduct Counts'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>CH2O2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ACN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CH3OH</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NH4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Na</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pos Adduct Counts'!$G$2:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0352</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0249</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1284407280"/>
+        <c:axId val="-1987147584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1284407280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1987147584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1987147584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1284407280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3063,20 +4975,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>746569</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>66504</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>115939</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3098,28 +6016,150 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_tran_counts" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_tran_counts" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_2_adduct_counts_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_adduct_counts_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_adduct_counts_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_adduct_counts_1" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_adduct_counts" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_adduct_counts" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_adduct_counts" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_2_adduct_counts" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_adduct_counts" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_adduct_counts" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_tran_counts" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_tran_counts" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_2_tran_counts" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_2_tran_counts" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_tran_counts" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_tran_counts" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_tran_counts" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_tran_counts" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_tran_counts" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_tran_counts" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_NEG_tran_counts" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_adduct_counts_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_adduct_counts_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3387,8 +6427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6399,4 +9439,1329 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3">
+        <v>1126</v>
+      </c>
+      <c r="C3">
+        <v>0.31780000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4">
+        <v>608</v>
+      </c>
+      <c r="C4">
+        <v>0.1716</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5">
+        <v>135</v>
+      </c>
+      <c r="C5">
+        <v>3.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6">
+        <v>122</v>
+      </c>
+      <c r="C6">
+        <v>3.44E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7">
+        <v>156</v>
+      </c>
+      <c r="C7">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>5.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13">
+        <v>256</v>
+      </c>
+      <c r="C13">
+        <v>7.2300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14">
+        <v>128</v>
+      </c>
+      <c r="C14">
+        <v>3.61E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15">
+        <v>140</v>
+      </c>
+      <c r="C15">
+        <v>3.95E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17">
+        <v>163</v>
+      </c>
+      <c r="C17">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>7.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31">
+        <v>95</v>
+      </c>
+      <c r="C31">
+        <v>2.6800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32">
+        <v>65</v>
+      </c>
+      <c r="C32">
+        <v>1.83E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33">
+        <v>58</v>
+      </c>
+      <c r="C33">
+        <v>1.6400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35">
+        <v>31</v>
+      </c>
+      <c r="C35">
+        <v>8.6999999999999994E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50">
+        <v>18</v>
+      </c>
+      <c r="C50">
+        <v>5.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51">
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54">
+        <v>63</v>
+      </c>
+      <c r="C54">
+        <v>1.78E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55">
+        <v>19</v>
+      </c>
+      <c r="C55">
+        <v>5.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56">
+        <v>39</v>
+      </c>
+      <c r="C56">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="7" width="7.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>7.6E-3</v>
+      </c>
+      <c r="D2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E2">
+        <v>1.15E-2</v>
+      </c>
+      <c r="F2">
+        <v>1.21E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.32E-2</v>
+      </c>
+      <c r="E3">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>3.5200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.41E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.14E-2</v>
+      </c>
+      <c r="E5">
+        <v>1.84E-2</v>
+      </c>
+      <c r="F5">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.63E-2</v>
+      </c>
+      <c r="F6">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.4899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.44E-2</v>
+      </c>
+      <c r="D7">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="E7">
+        <v>3.39E-2</v>
+      </c>
+      <c r="F7">
+        <v>3.1899999999999998E-2</v>
+      </c>
+      <c r="G7">
+        <v>3.4799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" t="s">
+        <v>152</v>
+      </c>
+      <c r="L12" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13">
+        <v>116</v>
+      </c>
+      <c r="C13">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="D13">
+        <v>49</v>
+      </c>
+      <c r="E13">
+        <v>7.6E-3</v>
+      </c>
+      <c r="F13">
+        <v>47</v>
+      </c>
+      <c r="G13">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H13">
+        <v>77</v>
+      </c>
+      <c r="I13">
+        <v>1.15E-2</v>
+      </c>
+      <c r="J13">
+        <v>80</v>
+      </c>
+      <c r="K13">
+        <v>1.21E-2</v>
+      </c>
+      <c r="L13">
+        <v>102</v>
+      </c>
+      <c r="M13">
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14">
+        <v>6938</v>
+      </c>
+      <c r="C14">
+        <v>0.83379999999999999</v>
+      </c>
+      <c r="D14">
+        <v>5677</v>
+      </c>
+      <c r="E14">
+        <v>0.88029999999999997</v>
+      </c>
+      <c r="F14">
+        <v>5181</v>
+      </c>
+      <c r="G14">
+        <v>0.88009999999999999</v>
+      </c>
+      <c r="H14">
+        <v>5798</v>
+      </c>
+      <c r="I14">
+        <v>0.86270000000000002</v>
+      </c>
+      <c r="J14">
+        <v>5778</v>
+      </c>
+      <c r="K14">
+        <v>0.87039999999999995</v>
+      </c>
+      <c r="L14">
+        <v>7019</v>
+      </c>
+      <c r="M14">
+        <v>0.85750000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15">
+        <v>299</v>
+      </c>
+      <c r="C15">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="D15">
+        <v>90</v>
+      </c>
+      <c r="E15">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F15">
+        <v>78</v>
+      </c>
+      <c r="G15">
+        <v>1.32E-2</v>
+      </c>
+      <c r="H15">
+        <v>179</v>
+      </c>
+      <c r="I15">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="J15">
+        <v>142</v>
+      </c>
+      <c r="K15">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="L15">
+        <v>288</v>
+      </c>
+      <c r="M15">
+        <v>3.5200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16">
+        <v>135</v>
+      </c>
+      <c r="C16">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="D16">
+        <v>136</v>
+      </c>
+      <c r="E16">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="F16">
+        <v>130</v>
+      </c>
+      <c r="G16">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="H16">
+        <v>138</v>
+      </c>
+      <c r="I16">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="J16">
+        <v>138</v>
+      </c>
+      <c r="K16">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="L16">
+        <v>115</v>
+      </c>
+      <c r="M16">
+        <v>1.41E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17">
+        <v>156</v>
+      </c>
+      <c r="C17">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="D17">
+        <v>84</v>
+      </c>
+      <c r="E17">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F17">
+        <v>67</v>
+      </c>
+      <c r="G17">
+        <v>1.14E-2</v>
+      </c>
+      <c r="H17">
+        <v>124</v>
+      </c>
+      <c r="I17">
+        <v>1.84E-2</v>
+      </c>
+      <c r="J17">
+        <v>116</v>
+      </c>
+      <c r="K17">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="L17">
+        <v>172</v>
+      </c>
+      <c r="M17">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18">
+        <v>267</v>
+      </c>
+      <c r="C18">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="D18">
+        <v>191</v>
+      </c>
+      <c r="E18">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="F18">
+        <v>180</v>
+      </c>
+      <c r="G18">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="H18">
+        <v>177</v>
+      </c>
+      <c r="I18">
+        <v>2.63E-2</v>
+      </c>
+      <c r="J18">
+        <v>172</v>
+      </c>
+      <c r="K18">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="L18">
+        <v>204</v>
+      </c>
+      <c r="M18">
+        <v>2.4899999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added output files, restructured output system
</commit_message>
<xml_diff>
--- a/notebooks/comparison_of_proportions_of_transformations_excluding_singletons.xlsx
+++ b/notebooks/comparison_of_proportions_of_transformations_excluding_singletons.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Positive mode" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="batch1_Std_2_2_tran_counts" localSheetId="0">'Positive mode'!$L$3:$M$73</definedName>
     <definedName name="Beer_3_Full1_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$A$2:$B$6</definedName>
     <definedName name="Beer_3_Full1_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$A$13:$C$18</definedName>
-    <definedName name="Beer_3_Full1_NEG_tran_counts" localSheetId="1">'Negative mode'!$A$3:$C$73</definedName>
+    <definedName name="Beer_3_Full1_NEG_tran_counts_1" localSheetId="1">'Negative mode'!$A$3:$C$73</definedName>
     <definedName name="Beer_3_Full1_tran_counts" localSheetId="0">'Positive mode'!$A$3:$C$73</definedName>
     <definedName name="Urine_37_fullscan1_POS_adduct_counts" localSheetId="2">'Pos Adduct Counts'!$G$2:$G$6</definedName>
     <definedName name="Urine_37_fullscan1_POS_adduct_counts_1" localSheetId="2">'Pos Adduct Counts'!$L$13:$M$18</definedName>
@@ -750,10 +750,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2716,11 +2716,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2070345584"/>
-        <c:axId val="-2037921648"/>
+        <c:axId val="-2104618960"/>
+        <c:axId val="-2104617376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2070345584"/>
+        <c:axId val="-2104618960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2763,7 +2763,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2037921648"/>
+        <c:crossAx val="-2104617376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2771,7 +2771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2037921648"/>
+        <c:axId val="-2104617376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2822,7 +2822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070345584"/>
+        <c:crossAx val="-2104618960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3207,103 +3207,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>0.3178</c:v>
+                  <c:v>0.3063</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1716</c:v>
+                  <c:v>0.1798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0381</c:v>
+                  <c:v>0.0487</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0344</c:v>
+                  <c:v>0.0402</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.044</c:v>
+                  <c:v>0.0329</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0045</c:v>
+                  <c:v>0.0046</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0014</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0051</c:v>
+                  <c:v>0.0043</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0034</c:v>
+                  <c:v>0.0139</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0723</c:v>
+                  <c:v>0.0472</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0361</c:v>
+                  <c:v>0.0576</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0395</c:v>
+                  <c:v>0.0422</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.004</c:v>
+                  <c:v>0.0228</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.046</c:v>
+                  <c:v>0.0209</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0008</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0085</c:v>
+                  <c:v>0.0081</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.0008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0031</c:v>
+                  <c:v>0.0073</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0023</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>0.005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.0046</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>0.0023</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>0.0008</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.013</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.004</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0079</c:v>
+                  <c:v>0.0081</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0268</c:v>
+                  <c:v>0.0259</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0183</c:v>
+                  <c:v>0.0139</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0164</c:v>
+                  <c:v>0.0124</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0056</c:v>
+                  <c:v>0.0058</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0087</c:v>
+                  <c:v>0.0089</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.0008</c:v>
@@ -3312,67 +3312,67 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0034</c:v>
+                  <c:v>0.0054</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0004</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0031</c:v>
+                  <c:v>0.0015</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0006</c:v>
+                  <c:v>0.0008</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0014</c:v>
+                  <c:v>0.0023</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0003</c:v>
+                  <c:v>0.0004</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0004</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0008</c:v>
+                  <c:v>0.0023</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0025</c:v>
+                  <c:v>0.0046</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0031</c:v>
+                  <c:v>0.0043</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0051</c:v>
+                  <c:v>0.0039</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0025</c:v>
+                  <c:v>0.0066</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0025</c:v>
+                  <c:v>0.0023</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0017</c:v>
+                  <c:v>0.0039</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0178</c:v>
+                  <c:v>0.0135</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>0.0054</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.011</c:v>
+                  <c:v>0.0073</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0004</c:v>
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>0.0</c:v>
@@ -3390,7 +3390,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0008</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>0.0</c:v>
@@ -3405,19 +3405,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0014</c:v>
+                  <c:v>0.0027</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.0003</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.0003</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.0006</c:v>
+                  <c:v>0.0004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3433,11 +3433,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2070310080"/>
-        <c:axId val="-2032344496"/>
+        <c:axId val="-2104563456"/>
+        <c:axId val="-2104559888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2070310080"/>
+        <c:axId val="-2104563456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3480,7 +3480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2032344496"/>
+        <c:crossAx val="-2104559888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3488,7 +3488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2032344496"/>
+        <c:axId val="-2104559888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3539,7 +3539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070310080"/>
+        <c:crossAx val="-2104563456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3660,7 +3660,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4175,11 +4174,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1284407280"/>
-        <c:axId val="-1987147584"/>
+        <c:axId val="2131213696"/>
+        <c:axId val="2131217008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1284407280"/>
+        <c:axId val="2131213696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4222,7 +4221,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1987147584"/>
+        <c:crossAx val="2131217008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4230,7 +4229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1987147584"/>
+        <c:axId val="2131217008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4281,7 +4280,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1284407280"/>
+        <c:crossAx val="2131213696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4295,7 +4294,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4773,11 +4771,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1289326592"/>
-        <c:axId val="1266087872"/>
+        <c:axId val="-2104526912"/>
+        <c:axId val="-2104523616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1289326592"/>
+        <c:axId val="-2104526912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4820,7 +4818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1266087872"/>
+        <c:crossAx val="-2104523616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4828,7 +4826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1266087872"/>
+        <c:axId val="-2104523616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4879,7 +4877,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1289326592"/>
+        <c:crossAx val="-2104526912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7273,51 +7271,51 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_tran_counts" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_tran_counts" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_adduct_counts" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_adduct_counts" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_2_adduct_counts" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_adduct_counts" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_adduct_counts" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_adduct_counts" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_adduct_counts_1" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_adduct_counts_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_adduct_counts_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_2_adduct_counts_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_adduct_counts_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_adduct_counts_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_adduct_counts_1" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_adduct_counts" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_adduct_counts" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_adduct_counts" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_2_adduct_counts" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_adduct_counts" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_adduct_counts" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_tran_counts" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_tran_counts" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7325,11 +7323,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_tran_counts" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_1_tran_counts" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Urine_37_fullscan1_POS_tran_counts" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_2_2_tran_counts" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7337,15 +7335,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_NEG_tran_counts" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_NEG_tran_counts_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_adduct_counts_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_adduct_counts_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="batch1_Std_1_1_adduct_counts_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Beer_3_Full1_adduct_counts_1" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7613,7 +7611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="93" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:M1"/>
     </sheetView>
   </sheetViews>
@@ -7636,30 +7634,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="1"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -10615,12 +10613,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10631,31 +10629,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -10664,10 +10662,10 @@
         <v>80</v>
       </c>
       <c r="B3">
-        <v>1126</v>
+        <v>792</v>
       </c>
       <c r="C3">
-        <v>0.31780000000000003</v>
+        <v>0.30630000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -10675,10 +10673,10 @@
         <v>81</v>
       </c>
       <c r="B4">
-        <v>608</v>
+        <v>465</v>
       </c>
       <c r="C4">
-        <v>0.1716</v>
+        <v>0.17979999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -10686,10 +10684,10 @@
         <v>82</v>
       </c>
       <c r="B5">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C5">
-        <v>3.8100000000000002E-2</v>
+        <v>4.87E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -10697,10 +10695,10 @@
         <v>83</v>
       </c>
       <c r="B6">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C6">
-        <v>3.44E-2</v>
+        <v>4.02E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -10708,10 +10706,10 @@
         <v>84</v>
       </c>
       <c r="B7">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="C7">
-        <v>4.3999999999999997E-2</v>
+        <v>3.2899999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -10719,10 +10717,10 @@
         <v>85</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>4.4999999999999997E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -10730,10 +10728,10 @@
         <v>86</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1.4E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -10741,10 +10739,10 @@
         <v>87</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>5.1000000000000004E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -10752,7 +10750,7 @@
         <v>88</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>8.0000000000000004E-4</v>
@@ -10763,10 +10761,10 @@
         <v>89</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C12">
-        <v>3.3999999999999998E-3</v>
+        <v>1.3899999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -10774,10 +10772,10 @@
         <v>90</v>
       </c>
       <c r="B13">
-        <v>256</v>
+        <v>122</v>
       </c>
       <c r="C13">
-        <v>7.2300000000000003E-2</v>
+        <v>4.7199999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -10785,10 +10783,10 @@
         <v>91</v>
       </c>
       <c r="B14">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="C14">
-        <v>3.61E-2</v>
+        <v>5.7599999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -10796,10 +10794,10 @@
         <v>92</v>
       </c>
       <c r="B15">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C15">
-        <v>3.95E-2</v>
+        <v>4.2200000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -10807,10 +10805,10 @@
         <v>93</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="C16">
-        <v>4.0000000000000001E-3</v>
+        <v>2.2800000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -10818,10 +10816,10 @@
         <v>94</v>
       </c>
       <c r="B17">
-        <v>163</v>
+        <v>54</v>
       </c>
       <c r="C17">
-        <v>4.5999999999999999E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -10829,10 +10827,10 @@
         <v>95</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -10851,10 +10849,10 @@
         <v>97</v>
       </c>
       <c r="B20">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C20">
-        <v>8.5000000000000006E-3</v>
+        <v>8.0999999999999996E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -10862,7 +10860,7 @@
         <v>98</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>8.0000000000000004E-4</v>
@@ -10873,10 +10871,10 @@
         <v>99</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>3.0999999999999999E-3</v>
+        <v>7.3000000000000001E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -10884,10 +10882,10 @@
         <v>100</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -10895,10 +10893,10 @@
         <v>101</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>2.3E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -10906,10 +10904,10 @@
         <v>102</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -10917,10 +10915,10 @@
         <v>103</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>4.5999999999999999E-3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -10928,10 +10926,10 @@
         <v>104</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C27">
-        <v>8.0000000000000004E-4</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -10939,10 +10937,10 @@
         <v>105</v>
       </c>
       <c r="B28">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>1.2999999999999999E-2</v>
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -10950,10 +10948,10 @@
         <v>106</v>
       </c>
       <c r="B29">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -10961,10 +10959,10 @@
         <v>107</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C30">
-        <v>7.9000000000000008E-3</v>
+        <v>8.0999999999999996E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -10972,10 +10970,10 @@
         <v>108</v>
       </c>
       <c r="B31">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C31">
-        <v>2.6800000000000001E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -10983,10 +10981,10 @@
         <v>109</v>
       </c>
       <c r="B32">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C32">
-        <v>1.83E-2</v>
+        <v>1.3899999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -10994,10 +10992,10 @@
         <v>110</v>
       </c>
       <c r="B33">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C33">
-        <v>1.6400000000000001E-2</v>
+        <v>1.24E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -11005,10 +11003,10 @@
         <v>111</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C34">
-        <v>5.5999999999999999E-3</v>
+        <v>5.7999999999999996E-3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -11016,10 +11014,10 @@
         <v>112</v>
       </c>
       <c r="B35">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C35">
-        <v>8.6999999999999994E-3</v>
+        <v>8.8999999999999999E-3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -11027,7 +11025,7 @@
         <v>113</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>8.0000000000000004E-4</v>
@@ -11049,10 +11047,10 @@
         <v>115</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C38">
-        <v>3.3999999999999998E-3</v>
+        <v>5.4000000000000003E-3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -11060,10 +11058,10 @@
         <v>116</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -11071,10 +11069,10 @@
         <v>117</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C40">
-        <v>3.0999999999999999E-3</v>
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -11085,7 +11083,7 @@
         <v>2</v>
       </c>
       <c r="C41">
-        <v>5.9999999999999995E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -11093,10 +11091,10 @@
         <v>119</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42">
-        <v>1.4E-3</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -11107,7 +11105,7 @@
         <v>1</v>
       </c>
       <c r="C43">
-        <v>2.9999999999999997E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -11115,10 +11113,10 @@
         <v>121</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -11137,10 +11135,10 @@
         <v>123</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>8.0000000000000004E-4</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -11159,10 +11157,10 @@
         <v>125</v>
       </c>
       <c r="B48">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>2.5000000000000001E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -11173,7 +11171,7 @@
         <v>11</v>
       </c>
       <c r="C49">
-        <v>3.0999999999999999E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -11181,10 +11179,10 @@
         <v>127</v>
       </c>
       <c r="B50">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>5.1000000000000004E-3</v>
+        <v>3.8999999999999998E-3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -11192,10 +11190,10 @@
         <v>128</v>
       </c>
       <c r="B51">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C51">
-        <v>2.5000000000000001E-3</v>
+        <v>6.6E-3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -11203,10 +11201,10 @@
         <v>129</v>
       </c>
       <c r="B52">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C52">
-        <v>2.5000000000000001E-3</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -11214,10 +11212,10 @@
         <v>130</v>
       </c>
       <c r="B53">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C53">
-        <v>1.6999999999999999E-3</v>
+        <v>3.8999999999999998E-3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -11225,10 +11223,10 @@
         <v>131</v>
       </c>
       <c r="B54">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C54">
-        <v>1.78E-2</v>
+        <v>1.35E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -11236,7 +11234,7 @@
         <v>132</v>
       </c>
       <c r="B55">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C55">
         <v>5.4000000000000003E-3</v>
@@ -11247,10 +11245,10 @@
         <v>133</v>
       </c>
       <c r="B56">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>1.0999999999999999E-2</v>
+        <v>7.3000000000000001E-3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -11269,10 +11267,10 @@
         <v>135</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -11335,10 +11333,10 @@
         <v>141</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -11390,10 +11388,10 @@
         <v>146</v>
       </c>
       <c r="B69">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>1.4E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -11401,10 +11399,10 @@
         <v>147</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>2.9999999999999997E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -11412,10 +11410,10 @@
         <v>148</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71">
-        <v>2.9999999999999997E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -11434,10 +11432,10 @@
         <v>150</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C73">
-        <v>5.9999999999999995E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
   </sheetData>
@@ -11468,22 +11466,22 @@
       <c r="A1" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -11626,30 +11624,30 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1" t="s">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="1"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -11940,12 +11938,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L11:M11"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11956,7 +11954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>

</xml_diff>